<commit_message>
HL update code for workflow 4
</commit_message>
<xml_diff>
--- a/Department/Department_List.xlsx
+++ b/Department/Department_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\UiPath\EmailAutomationRPA\Department\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PHAM HAI LONG\Documents\UiPath\EmailAutomationRPA\Department\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7E4AE3-9EB7-45F8-B09A-F753619F8611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EDFE0E-05EE-4EDE-B417-78D09FF22CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Customer Service</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>BD</t>
+  </si>
+  <si>
+    <t>Manager</t>
   </si>
 </sst>
 </file>
@@ -434,19 +437,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.81640625" customWidth="1"/>
+    <col min="1" max="1" width="27.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -454,7 +457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -462,7 +465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -470,7 +473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -478,7 +481,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -486,7 +489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -494,12 +497,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -510,6 +521,7 @@
     <hyperlink ref="A7" r:id="rId4" xr:uid="{1193CAB4-6175-4557-B414-A62EA8B355BC}"/>
     <hyperlink ref="A5" r:id="rId5" xr:uid="{D657A650-9DA9-4C73-9CA0-01326117B456}"/>
     <hyperlink ref="A3" r:id="rId6" xr:uid="{7988A62F-7A5A-4556-B6B8-9434263EF3C6}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{EF561B0A-BD14-44F5-B7FC-76526EB6026B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>